<commit_message>
tailored model, doesn't work
</commit_message>
<xml_diff>
--- a/data/generatorinfo.xlsx
+++ b/data/generatorinfo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/linaabedisa/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/linaabedisa/Documents/GitHub/AMO-Single-Project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EFD7FF7-1B10-8D47-AA63-D735983BB904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A6AE153-B7B5-0848-8563-902644A5070D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="500" windowWidth="19440" windowHeight="15920" xr2:uid="{0115F94E-3238-B04F-A64F-D694225D5EB6}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="16740" windowHeight="16140" xr2:uid="{0115F94E-3238-B04F-A64F-D694225D5EB6}"/>
   </bookViews>
   <sheets>
     <sheet name="generatorinfo" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>ID</t>
   </si>
@@ -53,169 +53,37 @@
     <t>g1</t>
   </si>
   <si>
-    <t>13.32</t>
-  </si>
-  <si>
-    <t>1.68</t>
-  </si>
-  <si>
-    <t>2.32</t>
-  </si>
-  <si>
-    <t>106.4</t>
-  </si>
-  <si>
-    <t>48</t>
-  </si>
-  <si>
     <t>g2</t>
   </si>
   <si>
     <t>g3</t>
   </si>
   <si>
-    <t>20.7</t>
-  </si>
-  <si>
-    <t>3.3</t>
-  </si>
-  <si>
-    <t>4.67</t>
-  </si>
-  <si>
-    <t>245</t>
-  </si>
-  <si>
-    <t>84</t>
-  </si>
-  <si>
     <t>g4</t>
   </si>
   <si>
-    <t>20.93</t>
-  </si>
-  <si>
-    <t>4.07</t>
-  </si>
-  <si>
-    <t>3.93</t>
-  </si>
-  <si>
-    <t>413.7</t>
-  </si>
-  <si>
-    <t>216</t>
-  </si>
-  <si>
     <t>g5</t>
   </si>
   <si>
-    <t>26.11</t>
-  </si>
-  <si>
-    <t>1.89</t>
-  </si>
-  <si>
-    <t>3.11</t>
-  </si>
-  <si>
-    <t>42</t>
-  </si>
-  <si>
     <t>g6</t>
   </si>
   <si>
-    <t>10.52</t>
-  </si>
-  <si>
-    <t>5.48</t>
-  </si>
-  <si>
-    <t>3.52</t>
-  </si>
-  <si>
-    <t>108.5</t>
-  </si>
-  <si>
-    <t>36</t>
-  </si>
-  <si>
     <t>g7</t>
   </si>
   <si>
     <t>g8</t>
   </si>
   <si>
-    <t>6.02</t>
-  </si>
-  <si>
-    <t>4.98</t>
-  </si>
-  <si>
-    <t>5.02</t>
-  </si>
-  <si>
-    <t>280</t>
-  </si>
-  <si>
-    <t>60</t>
-  </si>
-  <si>
     <t>g9</t>
   </si>
   <si>
-    <t>5.47</t>
-  </si>
-  <si>
-    <t>5.53</t>
-  </si>
-  <si>
-    <t>4.97</t>
-  </si>
-  <si>
     <t>g10</t>
   </si>
   <si>
-    <t>7.0</t>
-  </si>
-  <si>
-    <t>8.0</t>
-  </si>
-  <si>
-    <t>6.0</t>
-  </si>
-  <si>
-    <t>210.0</t>
-  </si>
-  <si>
-    <t>48.0</t>
-  </si>
-  <si>
     <t>g11</t>
   </si>
   <si>
-    <t>3.45</t>
-  </si>
-  <si>
-    <t>2.52</t>
-  </si>
-  <si>
-    <t>217</t>
-  </si>
-  <si>
-    <t>72</t>
-  </si>
-  <si>
     <t>g12</t>
-  </si>
-  <si>
-    <t>10.89</t>
-  </si>
-  <si>
-    <t>5.11</t>
-  </si>
-  <si>
-    <t>2.89</t>
   </si>
   <si>
     <t>upresercost</t>
@@ -263,9 +131,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -580,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{293AC1EB-083B-0E47-BEB0-3177B5E7A401}">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -592,7 +461,7 @@
     <col min="8" max="8" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -603,360 +472,412 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>60</v>
+        <v>16</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>61</v>
+        <v>17</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>62</v>
+        <v>18</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>63</v>
+        <v>19</v>
       </c>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>9</v>
+      <c r="C2" s="2">
+        <v>13.32</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1.68</v>
+      </c>
+      <c r="E2" s="2">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="F2" s="2">
+        <v>106.4</v>
+      </c>
+      <c r="G2" s="2">
+        <v>48</v>
+      </c>
+      <c r="H2" s="2">
+        <v>48</v>
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1">
         <v>2</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>9</v>
+      <c r="C3" s="2">
+        <v>13.32</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1.68</v>
+      </c>
+      <c r="E3" s="2">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="F3" s="2">
+        <v>106.4</v>
+      </c>
+      <c r="G3" s="2">
+        <v>48</v>
+      </c>
+      <c r="H3" s="2">
+        <v>48</v>
       </c>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B4" s="1">
         <v>7</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>16</v>
+      <c r="C4" s="2">
+        <v>20.7</v>
+      </c>
+      <c r="D4" s="2">
+        <v>3.3</v>
+      </c>
+      <c r="E4" s="2">
+        <v>4.67</v>
+      </c>
+      <c r="F4" s="2">
+        <v>245</v>
+      </c>
+      <c r="G4" s="2">
+        <v>84</v>
+      </c>
+      <c r="H4" s="2">
+        <v>84</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="B5" s="1">
         <v>13</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>22</v>
+      <c r="C5" s="2">
+        <v>20.93</v>
+      </c>
+      <c r="D5" s="2">
+        <v>4.07</v>
+      </c>
+      <c r="E5" s="2">
+        <v>3.93</v>
+      </c>
+      <c r="F5" s="2">
+        <v>413.7</v>
+      </c>
+      <c r="G5" s="2">
+        <v>216</v>
+      </c>
+      <c r="H5" s="2">
+        <v>216</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="B6" s="1">
         <v>15</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>27</v>
+      <c r="C6" s="2">
+        <v>26.11</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1.89</v>
+      </c>
+      <c r="E6" s="2">
+        <v>3.11</v>
+      </c>
+      <c r="F6" s="2">
+        <v>42</v>
+      </c>
+      <c r="G6" s="2">
+        <v>42</v>
+      </c>
+      <c r="H6" s="2">
+        <v>42</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="B7" s="1">
         <v>15</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>33</v>
+      <c r="C7" s="2">
+        <v>10.52</v>
+      </c>
+      <c r="D7" s="2">
+        <v>5.48</v>
+      </c>
+      <c r="E7" s="2">
+        <v>3.52</v>
+      </c>
+      <c r="F7" s="2">
+        <v>108.5</v>
+      </c>
+      <c r="G7" s="2">
+        <v>36</v>
+      </c>
+      <c r="H7" s="2">
+        <v>36</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="B8" s="1">
         <v>16</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>33</v>
+      <c r="C8" s="2">
+        <v>10.52</v>
+      </c>
+      <c r="D8" s="2">
+        <v>5.48</v>
+      </c>
+      <c r="E8" s="2">
+        <v>3.52</v>
+      </c>
+      <c r="F8" s="2">
+        <v>108.5</v>
+      </c>
+      <c r="G8" s="2">
+        <v>36</v>
+      </c>
+      <c r="H8" s="2">
+        <v>36</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="B9" s="1">
         <v>18</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>40</v>
+      <c r="C9" s="2">
+        <v>6.02</v>
+      </c>
+      <c r="D9" s="2">
+        <v>4.9800000000000004</v>
+      </c>
+      <c r="E9" s="2">
+        <v>5.0199999999999996</v>
+      </c>
+      <c r="F9" s="2">
+        <v>280</v>
+      </c>
+      <c r="G9" s="2">
+        <v>60</v>
+      </c>
+      <c r="H9" s="2">
+        <v>60</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>41</v>
+        <v>12</v>
       </c>
       <c r="B10" s="1">
         <v>21</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>40</v>
+      <c r="C10" s="2">
+        <v>5.47</v>
+      </c>
+      <c r="D10" s="2">
+        <v>5.53</v>
+      </c>
+      <c r="E10" s="2">
+        <v>4.97</v>
+      </c>
+      <c r="F10" s="2">
+        <v>280</v>
+      </c>
+      <c r="G10" s="2">
+        <v>60</v>
+      </c>
+      <c r="H10" s="2">
+        <v>60</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="B11" s="1">
         <v>22</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E11" s="1" t="s">
+      <c r="C11" s="2">
+        <v>7</v>
+      </c>
+      <c r="D11" s="2">
+        <v>8</v>
+      </c>
+      <c r="E11" s="2">
+        <v>6</v>
+      </c>
+      <c r="F11" s="2">
+        <v>210</v>
+      </c>
+      <c r="G11" s="2">
         <v>48</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>9</v>
+      <c r="H11" s="2">
+        <v>48</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>51</v>
+        <v>14</v>
       </c>
       <c r="B12" s="1">
         <v>23</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>55</v>
+      <c r="C12" s="2">
+        <v>10.52</v>
+      </c>
+      <c r="D12" s="2">
+        <v>3.45</v>
+      </c>
+      <c r="E12" s="2">
+        <v>2.52</v>
+      </c>
+      <c r="F12" s="2">
+        <v>217</v>
+      </c>
+      <c r="G12" s="2">
+        <v>72</v>
+      </c>
+      <c r="H12" s="2">
+        <v>72</v>
       </c>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>56</v>
+        <v>15</v>
       </c>
       <c r="B13" s="1">
         <v>23</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>9</v>
+      <c r="C13" s="2">
+        <v>10.89</v>
+      </c>
+      <c r="D13" s="2">
+        <v>5.1100000000000003</v>
+      </c>
+      <c r="E13" s="2">
+        <v>2.89</v>
+      </c>
+      <c r="F13" s="2">
+        <v>245</v>
+      </c>
+      <c r="G13" s="2">
+        <v>48</v>
+      </c>
+      <c r="H13" s="2">
+        <v>48</v>
       </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -968,7 +889,7 @@
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -980,7 +901,7 @@
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>

</xml_diff>